<commit_message>
db table problem fixed
</commit_message>
<xml_diff>
--- a/database/target.xlsx
+++ b/database/target.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="9">
   <si>
     <t>TONAME</t>
   </si>
@@ -852,9 +852,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:E97"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -941,6 +943,996 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>3</v>
+      </c>
+      <c r="E92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed check_for_subs function, serious login bug and authentication error in smtp sent to webhook
</commit_message>
<xml_diff>
--- a/database/target.xlsx
+++ b/database/target.xlsx
@@ -957,15 +957,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E28"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -975,187 +975,196 @@
       <c r="C1">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed filter not loading target file problem
</commit_message>
<xml_diff>
--- a/database/target.xlsx
+++ b/database/target.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>TONAME</t>
   </si>
@@ -27,22 +27,16 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Elva</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Daphne</t>
-  </si>
-  <si>
-    <t>Boone</t>
-  </si>
-  <si>
     <t>shahimrans64@gmail.com</t>
   </si>
   <si>
-    <t>shahimran@outlook.com</t>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Imran</t>
+  </si>
+  <si>
+    <t>shah_imran_sust@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -866,12 +860,12 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -897,47 +891,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
     <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="H5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>